<commit_message>
Started work on new tests
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Classes\SoftwareEngineering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Classes\SoftwareEngineering\Workspace\ClueGame\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C297B5B8-10E4-4A3E-B753-C630F1A17418}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6309842-FDAC-4E7E-BBC2-9FAE12754531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5955" xr2:uid="{8695571F-C914-46C7-BB9E-FE42745CB933}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8695571F-C914-46C7-BB9E-FE42745CB933}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="39">
   <si>
     <t>S</t>
   </si>
@@ -136,6 +147,12 @@
   </si>
   <si>
     <t>E*</t>
+  </si>
+  <si>
+    <t>adjacencywalkways</t>
+  </si>
+  <si>
+    <t>room test</t>
   </si>
 </sst>
 </file>
@@ -151,7 +168,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,6 +211,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -207,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -215,6 +244,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,15 +560,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C948FBA-8EF7-4A7A-8713-7BE830607364}">
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="4.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="27" max="27" width="27.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>0</v>
       </c>
@@ -634,7 +668,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>0</f>
         <v>0</v>
@@ -711,8 +745,11 @@
       <c r="Y2" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="AA2" s="7" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>A2+1</f>
         <v>1</v>
@@ -789,8 +826,11 @@
       <c r="Y3" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="AA3" s="8" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" ref="A4:A25" si="1">A3+1</f>
         <v>2</v>
@@ -868,7 +908,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -939,14 +979,14 @@
       <c r="W5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="X5" s="2" t="s">
+      <c r="X5" s="7" t="s">
         <v>13</v>
       </c>
       <c r="Y5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -1024,7 +1064,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -1102,7 +1142,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -1180,7 +1220,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -1258,12 +1298,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1332,11 +1372,11 @@
       <c r="X10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Y10" s="5" t="s">
+      <c r="Y10" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -1404,7 +1444,7 @@
       <c r="V11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="W11" s="1" t="s">
+      <c r="W11" s="8" t="s">
         <v>0</v>
       </c>
       <c r="X11" s="1" t="s">
@@ -1414,7 +1454,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -1492,7 +1532,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -1570,7 +1610,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -1648,7 +1688,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1726,7 +1766,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1737,7 +1777,7 @@
       <c r="C16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -1804,7 +1844,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1882,7 +1922,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1960,7 +2000,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -2038,7 +2078,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -2116,7 +2156,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -2194,7 +2234,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -2272,7 +2312,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -2350,7 +2390,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -2428,7 +2468,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="1"/>
         <v>23</v>

</xml_diff>

<commit_message>
Added color key for tests on file
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Classes\SoftwareEngineering\Workspace\ClueGame\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6309842-FDAC-4E7E-BBC2-9FAE12754531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD530385-9C1A-48F7-B539-4AB853B24F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8695571F-C914-46C7-BB9E-FE42745CB933}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="40">
   <si>
     <t>S</t>
   </si>
@@ -152,7 +152,10 @@
     <t>adjacencywalkways</t>
   </si>
   <si>
-    <t>room test</t>
+    <t>testTargets</t>
+  </si>
+  <si>
+    <t>testOccupied</t>
   </si>
 </sst>
 </file>
@@ -168,7 +171,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,7 +222,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.499984740745262"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -236,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -246,6 +255,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,7 +573,7 @@
   <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="AB17" sqref="AB17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -907,6 +917,9 @@
       <c r="Y4" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="AA4" s="9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -943,7 +956,7 @@
       <c r="K5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="8" t="s">
         <v>22</v>
       </c>
       <c r="M5" s="1" t="s">
@@ -1315,7 +1328,7 @@
       <c r="E10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="8" t="s">
         <v>25</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -1444,7 +1457,7 @@
       <c r="V11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="W11" s="8" t="s">
+      <c r="W11" s="7" t="s">
         <v>0</v>
       </c>
       <c r="X11" s="1" t="s">
@@ -1489,7 +1502,7 @@
       <c r="K12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="L12" s="8" t="s">
         <v>17</v>
       </c>
       <c r="M12" s="2" t="s">
@@ -1738,7 +1751,7 @@
       <c r="P15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q15" s="5" t="s">
+      <c r="Q15" s="8" t="s">
         <v>16</v>
       </c>
       <c r="R15" s="1" t="s">
@@ -1759,10 +1772,10 @@
       <c r="W15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="X15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y15" s="2" t="s">
+      <c r="X15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y15" s="8" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1801,7 +1814,7 @@
       <c r="K16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L16" s="6" t="s">
+      <c r="L16" s="9" t="s">
         <v>29</v>
       </c>
       <c r="M16" s="1" t="s">
@@ -2023,7 +2036,7 @@
       <c r="G19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H19" s="9" t="s">
         <v>17</v>
       </c>
       <c r="I19" s="2" t="s">
@@ -2197,13 +2210,13 @@
       <c r="M21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N21" s="5" t="s">
+      <c r="N21" s="9" t="s">
         <v>16</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="P21" s="6" t="s">
+      <c r="P21" s="8" t="s">
         <v>36</v>
       </c>
       <c r="Q21" s="1" t="s">
@@ -2410,7 +2423,7 @@
       <c r="F24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H24" s="2" t="s">
@@ -2548,5 +2561,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add board with players and rooms and room names.
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Classes\SoftwareEngineering\Workspace\ClueGame\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dawso\eclipse-workspace\ClueGame\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD530385-9C1A-48F7-B539-4AB853B24F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7268CB-BCFA-4E25-8777-C3A8F2AA281F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8695571F-C914-46C7-BB9E-FE42745CB933}"/>
   </bookViews>
@@ -573,7 +573,7 @@
   <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB17" sqref="AB17"/>
+      <selection activeCell="X21" sqref="X21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -848,11 +848,11 @@
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>8</v>
@@ -872,11 +872,11 @@
       <c r="J4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L4" s="6" t="s">
+      <c r="K4" s="6" t="s">
         <v>21</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>9</v>
@@ -896,11 +896,11 @@
       <c r="R4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="T4" s="6" t="s">
+      <c r="S4" s="6" t="s">
         <v>24</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="U4" s="1" t="s">
         <v>6</v>
@@ -1325,47 +1325,47 @@
       <c r="D10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" s="8" t="s">
+      <c r="E10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R10" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R10" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="S10" s="1" t="s">
         <v>0</v>
@@ -1706,14 +1706,14 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>4</v>
+      <c r="B15" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>28</v>
+      <c r="D15" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>4</v>
@@ -1730,14 +1730,14 @@
       <c r="I15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>10</v>
+      <c r="J15" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L15" s="6" t="s">
-        <v>30</v>
+      <c r="L15" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>10</v>
@@ -1754,14 +1754,14 @@
       <c r="Q15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="R15" s="1" t="s">
-        <v>11</v>
+      <c r="R15" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="S15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="T15" s="6" t="s">
-        <v>32</v>
+      <c r="T15" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="U15" s="1" t="s">
         <v>11</v>
@@ -2177,32 +2177,32 @@
       <c r="B21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="6" t="s">
+      <c r="C21" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K21" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>12</v>
@@ -2213,8 +2213,8 @@
       <c r="N21" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="O21" s="1" t="s">
-        <v>1</v>
+      <c r="O21" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="P21" s="8" t="s">
         <v>36</v>
@@ -2231,8 +2231,8 @@
       <c r="T21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="U21" s="6" t="s">
-        <v>35</v>
+      <c r="U21" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="V21" s="1" t="s">
         <v>1</v>

</xml_diff>